<commit_message>
Further added chnage to 1.5
</commit_message>
<xml_diff>
--- a/data/fabian/output/processed_f.xlsx
+++ b/data/fabian/output/processed_f.xlsx
@@ -536,7 +536,7 @@
         <v>50.21</v>
       </c>
       <c r="E2" t="n">
-        <v>0.61</v>
+        <v>0.41</v>
       </c>
       <c r="F2" t="n">
         <v>-55.96</v>
@@ -548,7 +548,7 @@
         <v>50.21</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="J2" t="n">
         <v>-41</v>
@@ -560,7 +560,7 @@
         <v>50.21</v>
       </c>
       <c r="M2" t="n">
-        <v>1.22</v>
+        <v>0.82</v>
       </c>
       <c r="N2" t="n">
         <v>43392.34</v>
@@ -591,7 +591,7 @@
         <v>50.21</v>
       </c>
       <c r="E3" t="n">
-        <v>0.54</v>
+        <v>0.36</v>
       </c>
       <c r="F3" t="n">
         <v>-60.71</v>
@@ -603,7 +603,7 @@
         <v>50.21</v>
       </c>
       <c r="I3" t="n">
-        <v>0.83</v>
+        <v>0.55</v>
       </c>
       <c r="J3" t="n">
         <v>-46.25</v>
@@ -615,7 +615,7 @@
         <v>50.21</v>
       </c>
       <c r="M3" t="n">
-        <v>1.09</v>
+        <v>0.72</v>
       </c>
       <c r="N3" t="n">
         <v>43392.34</v>
@@ -646,7 +646,7 @@
         <v>50.21</v>
       </c>
       <c r="E4" t="n">
-        <v>0.54</v>
+        <v>0.36</v>
       </c>
       <c r="F4" t="n">
         <v>-60.88</v>
@@ -658,7 +658,7 @@
         <v>50.21</v>
       </c>
       <c r="I4" t="n">
-        <v>0.82</v>
+        <v>0.55</v>
       </c>
       <c r="J4" t="n">
         <v>-46.1</v>
@@ -670,7 +670,7 @@
         <v>50.21</v>
       </c>
       <c r="M4" t="n">
-        <v>1.09</v>
+        <v>0.73</v>
       </c>
       <c r="N4" t="n">
         <v>43392.34</v>
@@ -701,7 +701,7 @@
         <v>50.21</v>
       </c>
       <c r="E5" t="n">
-        <v>0.55</v>
+        <v>0.37</v>
       </c>
       <c r="F5" t="n">
         <v>-60.72</v>
@@ -713,7 +713,7 @@
         <v>50.21</v>
       </c>
       <c r="I5" t="n">
-        <v>0.83</v>
+        <v>0.55</v>
       </c>
       <c r="J5" t="n">
         <v>-45.83</v>
@@ -725,7 +725,7 @@
         <v>50.21</v>
       </c>
       <c r="M5" t="n">
-        <v>1.1</v>
+        <v>0.73</v>
       </c>
       <c r="N5" t="n">
         <v>43392.34</v>
@@ -756,7 +756,7 @@
         <v>50.21</v>
       </c>
       <c r="E6" t="n">
-        <v>0.55</v>
+        <v>0.37</v>
       </c>
       <c r="F6" t="n">
         <v>-60.59</v>
@@ -768,7 +768,7 @@
         <v>50.21</v>
       </c>
       <c r="I6" t="n">
-        <v>0.83</v>
+        <v>0.55</v>
       </c>
       <c r="J6" t="n">
         <v>-45.72</v>
@@ -780,7 +780,7 @@
         <v>50.21</v>
       </c>
       <c r="M6" t="n">
-        <v>1.1</v>
+        <v>0.73</v>
       </c>
       <c r="N6" t="n">
         <v>43392.34</v>
@@ -811,7 +811,7 @@
         <v>50.21</v>
       </c>
       <c r="E7" t="n">
-        <v>0.55</v>
+        <v>0.37</v>
       </c>
       <c r="F7" t="n">
         <v>-60.72</v>
@@ -823,7 +823,7 @@
         <v>50.21</v>
       </c>
       <c r="I7" t="n">
-        <v>0.83</v>
+        <v>0.55</v>
       </c>
       <c r="J7" t="n">
         <v>-45.83</v>
@@ -835,7 +835,7 @@
         <v>50.21</v>
       </c>
       <c r="M7" t="n">
-        <v>1.1</v>
+        <v>0.73</v>
       </c>
       <c r="N7" t="n">
         <v>43392.34</v>
@@ -866,7 +866,7 @@
         <v>50.21</v>
       </c>
       <c r="E8" t="n">
-        <v>0.54</v>
+        <v>0.36</v>
       </c>
       <c r="F8" t="n">
         <v>-60.88</v>
@@ -878,7 +878,7 @@
         <v>50.21</v>
       </c>
       <c r="I8" t="n">
-        <v>0.82</v>
+        <v>0.55</v>
       </c>
       <c r="J8" t="n">
         <v>-46.1</v>
@@ -890,7 +890,7 @@
         <v>50.21</v>
       </c>
       <c r="M8" t="n">
-        <v>1.09</v>
+        <v>0.73</v>
       </c>
       <c r="N8" t="n">
         <v>43392.34</v>
@@ -921,7 +921,7 @@
         <v>50.21</v>
       </c>
       <c r="E9" t="n">
-        <v>0.54</v>
+        <v>0.36</v>
       </c>
       <c r="F9" t="n">
         <v>-60.71</v>
@@ -933,7 +933,7 @@
         <v>50.21</v>
       </c>
       <c r="I9" t="n">
-        <v>0.83</v>
+        <v>0.55</v>
       </c>
       <c r="J9" t="n">
         <v>-46.25</v>
@@ -945,7 +945,7 @@
         <v>50.21</v>
       </c>
       <c r="M9" t="n">
-        <v>1.09</v>
+        <v>0.72</v>
       </c>
       <c r="N9" t="n">
         <v>43392.34</v>
@@ -976,7 +976,7 @@
         <v>50.21</v>
       </c>
       <c r="E10" t="n">
-        <v>0.61</v>
+        <v>0.41</v>
       </c>
       <c r="F10" t="n">
         <v>-55.96</v>
@@ -988,7 +988,7 @@
         <v>50.21</v>
       </c>
       <c r="I10" t="n">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="J10" t="n">
         <v>-41</v>
@@ -1000,7 +1000,7 @@
         <v>50.21</v>
       </c>
       <c r="M10" t="n">
-        <v>1.22</v>
+        <v>0.82</v>
       </c>
       <c r="N10" t="n">
         <v>43392.34</v>

</xml_diff>